<commit_message>
defect log, project report and test report updated
</commit_message>
<xml_diff>
--- a/Defect Tracking log.xlsx
+++ b/Defect Tracking log.xlsx
@@ -5,23 +5,23 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Software Testing\TCSion\TCS Internship Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Software Testing\TCSion\Try 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{526A8B4E-1E20-4ECF-8EA0-607B145A6309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BACC883-335B-47E2-8658-5911D6AC826B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23880" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Defect Tracking log" sheetId="1" r:id="rId1"/>
     <sheet name="Screenshots" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="64">
   <si>
     <t>DEFECT TRACKING LOG</t>
   </si>
@@ -203,6 +203,39 @@
   <si>
     <t>Booking counts not displayed</t>
   </si>
+  <si>
+    <t>DEF-1</t>
+  </si>
+  <si>
+    <t>DEF-2</t>
+  </si>
+  <si>
+    <t>DEF-3</t>
+  </si>
+  <si>
+    <t>DEF-4</t>
+  </si>
+  <si>
+    <t>DEF-5</t>
+  </si>
+  <si>
+    <t>DEF-6</t>
+  </si>
+  <si>
+    <t>DEF-7</t>
+  </si>
+  <si>
+    <t>DEF-8</t>
+  </si>
+  <si>
+    <t>DEF-9</t>
+  </si>
+  <si>
+    <t>DEF-10</t>
+  </si>
+  <si>
+    <t>DEF-11</t>
+  </si>
 </sst>
 </file>
 
@@ -211,7 +244,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\-mmm\-yyyy"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -263,6 +296,11 @@
       <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -838,8 +876,8 @@
   </sheetPr>
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -862,7 +900,7 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -874,7 +912,7 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -913,8 +951,8 @@
       <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
-        <v>1</v>
+      <c r="A5" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="B5" s="4">
         <v>44847</v>
@@ -939,8 +977,8 @@
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
-        <v>2</v>
+      <c r="A6" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="B6" s="4">
         <v>44854</v>
@@ -965,8 +1003,8 @@
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
-        <v>3</v>
+      <c r="A7" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="B7" s="4">
         <v>44854</v>
@@ -991,8 +1029,8 @@
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
-        <v>4</v>
+      <c r="A8" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="B8" s="4">
         <v>44857</v>
@@ -1017,8 +1055,8 @@
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
-        <v>5</v>
+      <c r="A9" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="B9" s="4">
         <v>44860</v>
@@ -1043,8 +1081,8 @@
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
-        <v>6</v>
+      <c r="A10" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="B10" s="4">
         <v>44861</v>
@@ -1069,8 +1107,8 @@
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
-        <v>7</v>
+      <c r="A11" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="B11" s="4">
         <v>44861</v>
@@ -1095,8 +1133,8 @@
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
-        <v>8</v>
+      <c r="A12" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="B12" s="4">
         <v>44861</v>
@@ -1121,8 +1159,8 @@
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
-        <v>9</v>
+      <c r="A13" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="B13" s="4">
         <v>44861</v>
@@ -1147,8 +1185,8 @@
       <c r="J13" s="1"/>
     </row>
     <row r="14" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
-        <v>10</v>
+      <c r="A14" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="B14" s="4">
         <v>44864</v>
@@ -1173,8 +1211,8 @@
       <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A15" s="3">
-        <v>11</v>
+      <c r="A15" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="B15" s="4">
         <v>44868</v>
@@ -1286,6 +1324,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>
+  <phoneticPr fontId="9" type="noConversion"/>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" sqref="F5:F21" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"High,Medium,Low"</formula1>

</xml_diff>